<commit_message>
script and data update
update new script for chart reliability. New excel file for latest participant batch
</commit_message>
<xml_diff>
--- a/analysis/SubIDs.xlsx
+++ b/analysis/SubIDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABYTE\AppData\LocalLow\Rokers Vision Lab\Vision VR\Ben-s-capstone-data-analysis\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7DF19B-3923-4971-90FE-F94B7CA2F18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78913FE-9FFF-4964-9C1C-BAD5F33C62B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -125,8 +125,15 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,8 +152,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -154,11 +167,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -182,6 +210,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -195,6 +232,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,55 +458,55 @@
   <dimension ref="A1:K997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="15" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
@@ -716,7 +758,7 @@
       </c>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>9</v>
       </c>
@@ -736,17 +778,59 @@
       </c>
       <c r="J12" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="I14" s="9"/>
+    <row r="13" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24">
+        <v>10</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17">
+        <v>-0.18</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17">
+        <v>-0.1</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24">
+        <v>11</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="G14" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17">
+        <v>-0.08</v>
+      </c>
+      <c r="J14" s="15">
+        <v>0.98</v>
+      </c>
+      <c r="K14" s="16"/>
     </row>
     <row r="15" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>

</xml_diff>